<commit_message>
Implemented 4 file input buttons, separated nodes, connections and data bindings, xml generation with dummy pid-connections.json
</commit_message>
<xml_diff>
--- a/3 Entwicklungsphase/pid-instances.xlsx
+++ b/3 Entwicklungsphase/pid-instances.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel.romero.karam\Google Drive\TUM\Maschinenwesen B.Sc\Bachelorarbeit\3 Entwicklungsphase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Google Drive\TUM\Maschinenwesen B.Sc\Bachelorarbeit\3 Entwicklungsphase\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5286D3-52F1-4BFE-BA7B-116E157C41AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="u0ni0-7sw2i" sheetId="1" r:id="rId1"/>
@@ -398,9 +399,6 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>P&amp;ID Verteci Instances in AIS Visualization</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -411,12 +409,15 @@
   </si>
   <si>
     <t>Visualization Data</t>
+  </si>
+  <si>
+    <t>P&amp;ID Node Instances in AIS Visualization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -774,9 +775,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -811,18 +809,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -856,9 +842,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1140,54 +1141,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.71875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.71875" style="3" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
     <col min="5" max="5" width="15" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" customWidth="1"/>
-    <col min="8" max="10" width="20.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="32.28515625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="1029" width="11.5703125"/>
+    <col min="8" max="10" width="20.44140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="32.27734375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="10.71875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="1029" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="20.100000000000001" x14ac:dyDescent="0.7">
+      <c r="A1" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+    </row>
+    <row r="2" spans="1:15" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1204,111 +1205,111 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+    <row r="3" spans="1:15" ht="15.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="33"/>
-    </row>
-    <row r="4" spans="1:15" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="36" t="s">
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50"/>
+    </row>
+    <row r="4" spans="1:15" s="6" customFormat="1" ht="15.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="46"/>
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="J4" s="40" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="49" t="s">
+      <c r="O4" s="44" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="24">
         <v>1</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="37" t="s">
+      <c r="B5" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="44" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="46"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="50"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
+      <c r="M5" s="41"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="45"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" s="24">
         <v>2</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1326,12 +1327,12 @@
       <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="13"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="12"/>
       <c r="L6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1339,13 +1340,13 @@
         <v>22</v>
       </c>
       <c r="N6" s="11"/>
-      <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="25">
+      <c r="O6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="24">
         <v>3</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1363,24 +1364,24 @@
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="13"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="11"/>
-      <c r="O7" s="17"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="25">
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="24">
         <v>4</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1398,12 +1399,12 @@
       <c r="G8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="13" t="s">
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L8" s="4" t="s">
@@ -1413,15 +1414,15 @@
       <c r="N8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="16">
         <v>4000</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="24">
         <v>5</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1439,12 +1440,12 @@
       <c r="G9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="13" t="s">
+      <c r="I9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L9" s="4" t="s">
@@ -1454,15 +1455,15 @@
       <c r="N9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="16">
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="24">
         <v>6</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1480,24 +1481,24 @@
       <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="25">
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="24">
         <v>7</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1515,12 +1516,12 @@
       <c r="G11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="13"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1528,13 +1529,13 @@
         <v>41</v>
       </c>
       <c r="N11" s="11"/>
-      <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="25">
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" s="24">
         <v>8</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1552,24 +1553,24 @@
       <c r="G12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="17"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="24">
         <v>9</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1587,12 +1588,12 @@
       <c r="G13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13" t="s">
+      <c r="I13" s="15"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L13" s="4" t="s">
@@ -1602,15 +1603,15 @@
       <c r="N13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="16">
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="24">
         <v>10</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1628,12 +1629,12 @@
       <c r="G14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13" t="s">
+      <c r="I14" s="15"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L14" s="4" t="s">
@@ -1643,15 +1644,15 @@
       <c r="N14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="16">
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" s="24">
         <v>11</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1669,12 +1670,12 @@
       <c r="G15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13" t="s">
+      <c r="I15" s="15"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L15" s="4" t="s">
@@ -1684,15 +1685,15 @@
       <c r="N15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="16">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="25">
-        <v>12</v>
-      </c>
-      <c r="B16" s="26" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="24">
+        <v>12</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1710,24 +1711,24 @@
       <c r="G16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="11"/>
-      <c r="O16" s="17"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="25">
-        <v>13</v>
-      </c>
-      <c r="B17" s="26" t="s">
+      <c r="O16" s="16"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A17" s="24">
+        <v>13</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1745,24 +1746,24 @@
       <c r="G17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="11"/>
-      <c r="O17" s="17"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="25">
-        <v>14</v>
-      </c>
-      <c r="B18" s="26" t="s">
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A18" s="24">
+        <v>14</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1780,24 +1781,24 @@
       <c r="G18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="17"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="25">
+      <c r="O18" s="16"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A19" s="24">
         <v>15</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1815,24 +1816,24 @@
       <c r="G19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="13"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="17"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="25">
+      <c r="O19" s="16"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A20" s="24">
         <v>16</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1850,24 +1851,24 @@
       <c r="G20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="11"/>
-      <c r="O20" s="17"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="25">
+      <c r="O20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A21" s="24">
         <v>17</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1885,24 +1886,24 @@
       <c r="G21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="13"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="12"/>
       <c r="L21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="11"/>
-      <c r="O21" s="17"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="25">
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A22" s="24">
         <v>18</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1920,24 +1921,24 @@
       <c r="G22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="13"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="11"/>
-      <c r="O22" s="17"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="25">
+      <c r="O22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A23" s="24">
         <v>19</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1955,24 +1956,24 @@
       <c r="G23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="13"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="11"/>
-      <c r="O23" s="17"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="25">
+      <c r="O23" s="16"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A24" s="24">
         <v>20</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1990,24 +1991,24 @@
       <c r="G24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="13"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="12"/>
       <c r="L24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="11"/>
-      <c r="O24" s="17"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="25">
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A25" s="24">
         <v>21</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2025,24 +2026,24 @@
       <c r="G25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="16"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="13"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="17"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="25">
+      <c r="O25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A26" s="24">
         <v>22</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -2060,24 +2061,24 @@
       <c r="G26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="13"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="12"/>
       <c r="L26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="11"/>
-      <c r="O26" s="17"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="25">
+      <c r="O26" s="16"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A27" s="24">
         <v>23</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -2095,12 +2096,12 @@
       <c r="G27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="27" t="s">
+      <c r="H27" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="I27" s="16"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="13"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="12"/>
       <c r="L27" s="4" t="s">
         <v>73</v>
       </c>
@@ -2108,15 +2109,15 @@
       <c r="N27" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O27" s="17">
+      <c r="O27" s="16">
         <v>3000</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A28" s="24">
         <v>24</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -2134,24 +2135,24 @@
       <c r="G28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H28" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="I28" s="16"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="13"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="12"/>
       <c r="L28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="11"/>
-      <c r="O28" s="17"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="25">
+      <c r="O28" s="16"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A29" s="24">
         <v>25</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -2169,24 +2170,24 @@
       <c r="G29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H29" s="27" t="s">
+      <c r="H29" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="13"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="12"/>
       <c r="L29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="11"/>
-      <c r="O29" s="17"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="25">
+      <c r="O29" s="16"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A30" s="24">
         <v>26</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -2204,24 +2205,24 @@
       <c r="G30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="27" t="s">
+      <c r="H30" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="13"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="12"/>
       <c r="L30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="11"/>
-      <c r="O30" s="17"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="25">
+      <c r="O30" s="16"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A31" s="24">
         <v>27</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2239,24 +2240,24 @@
       <c r="G31" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H31" s="27" t="s">
+      <c r="H31" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="13"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="12"/>
       <c r="L31" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="11"/>
-      <c r="O31" s="17"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="25">
+      <c r="O31" s="16"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A32" s="24">
         <v>28</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -2274,24 +2275,24 @@
       <c r="G32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H32" s="27" t="s">
+      <c r="H32" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="13"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="12"/>
       <c r="L32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="11"/>
-      <c r="O32" s="17"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="25">
+      <c r="O32" s="16"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A33" s="24">
         <v>29</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2309,24 +2310,24 @@
       <c r="G33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H33" s="27" t="s">
+      <c r="H33" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="I33" s="16"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="13"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="12"/>
       <c r="L33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="11"/>
-      <c r="O33" s="17"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="25">
+      <c r="O33" s="16"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A34" s="24">
         <v>30</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2344,24 +2345,24 @@
       <c r="G34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H34" s="27" t="s">
+      <c r="H34" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="13"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="12"/>
       <c r="L34" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="11"/>
-      <c r="O34" s="17"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="25">
+      <c r="O34" s="16"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A35" s="24">
         <v>31</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -2379,12 +2380,12 @@
       <c r="G35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H35" s="27" t="s">
+      <c r="H35" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="13"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="12"/>
       <c r="L35" s="4" t="s">
         <v>19</v>
       </c>
@@ -2392,13 +2393,13 @@
         <v>94</v>
       </c>
       <c r="N35" s="11"/>
-      <c r="O35" s="17"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="25">
+      <c r="O35" s="16"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A36" s="24">
         <v>32</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -2416,24 +2417,24 @@
       <c r="G36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H36" s="27" t="s">
+      <c r="H36" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="13"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="12"/>
       <c r="L36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M36" s="10"/>
       <c r="N36" s="11"/>
-      <c r="O36" s="17"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="25">
+      <c r="O36" s="16"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A37" s="24">
         <v>33</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -2451,24 +2452,24 @@
       <c r="G37" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H37" s="27" t="s">
+      <c r="H37" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="13"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="12"/>
       <c r="L37" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M37" s="10"/>
       <c r="N37" s="11"/>
-      <c r="O37" s="17"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="25">
+      <c r="O37" s="16"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A38" s="24">
         <v>34</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -2486,12 +2487,12 @@
       <c r="G38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H38" s="27" t="s">
+      <c r="H38" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="I38" s="16"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="13"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="12"/>
       <c r="L38" s="4" t="s">
         <v>102</v>
       </c>
@@ -2499,15 +2500,15 @@
       <c r="N38" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="O38" s="17">
+      <c r="O38" s="16">
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A39" s="24">
         <v>35</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -2525,12 +2526,12 @@
       <c r="G39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H39" s="27" t="s">
+      <c r="H39" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I39" s="16"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="13"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="12"/>
       <c r="L39" s="4" t="s">
         <v>73</v>
       </c>
@@ -2538,15 +2539,15 @@
       <c r="N39" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O39" s="17">
+      <c r="O39" s="16">
         <v>2000</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A40" s="24">
         <v>36</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -2564,24 +2565,24 @@
       <c r="G40" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H40" s="27" t="s">
+      <c r="H40" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="I40" s="16"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="13"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="12"/>
       <c r="L40" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M40" s="10"/>
       <c r="N40" s="11"/>
-      <c r="O40" s="17"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="25">
+      <c r="O40" s="16"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A41" s="24">
         <v>37</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2599,24 +2600,24 @@
       <c r="G41" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H41" s="27" t="s">
+      <c r="H41" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="I41" s="16"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="13"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="12"/>
       <c r="L41" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M41" s="10"/>
       <c r="N41" s="11"/>
-      <c r="O41" s="17"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="25">
+      <c r="O41" s="16"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A42" s="24">
         <v>38</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -2634,24 +2635,24 @@
       <c r="G42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H42" s="27" t="s">
+      <c r="H42" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="13"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="12"/>
       <c r="L42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M42" s="10"/>
       <c r="N42" s="11"/>
-      <c r="O42" s="17"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="25">
+      <c r="O42" s="16"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A43" s="24">
         <v>39</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -2669,24 +2670,24 @@
       <c r="G43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H43" s="27" t="s">
+      <c r="H43" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="13"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="12"/>
       <c r="L43" s="4" t="s">
         <v>11</v>
       </c>
       <c r="M43" s="10"/>
       <c r="N43" s="11"/>
-      <c r="O43" s="17"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="25">
+      <c r="O43" s="16"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A44" s="24">
         <v>40</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -2702,22 +2703,22 @@
         <v>24</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="13"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="12"/>
       <c r="L44" s="4" t="s">
         <v>116</v>
       </c>
       <c r="M44" s="10"/>
       <c r="N44" s="11"/>
-      <c r="O44" s="17"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="25">
+      <c r="O44" s="16"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A45" s="24">
         <v>41</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -2733,22 +2734,22 @@
         <v>24</v>
       </c>
       <c r="G45" s="2"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="13"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="12"/>
       <c r="L45" s="4" t="s">
         <v>117</v>
       </c>
       <c r="M45" s="10"/>
       <c r="N45" s="11"/>
-      <c r="O45" s="17"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="25">
+      <c r="O45" s="16"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A46" s="24">
         <v>42</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -2764,22 +2765,22 @@
         <v>24</v>
       </c>
       <c r="G46" s="2"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="13"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="12"/>
       <c r="L46" s="4" t="s">
         <v>118</v>
       </c>
       <c r="M46" s="10"/>
       <c r="N46" s="11"/>
-      <c r="O46" s="17"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="25">
+      <c r="O46" s="16"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A47" s="24">
         <v>43</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -2795,22 +2796,22 @@
         <v>35</v>
       </c>
       <c r="G47" s="2"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="13"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="12"/>
       <c r="L47" s="4" t="s">
         <v>119</v>
       </c>
       <c r="M47" s="10"/>
       <c r="N47" s="11"/>
-      <c r="O47" s="17"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="25">
+      <c r="O47" s="16"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A48" s="24">
         <v>44</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -2826,10 +2827,10 @@
         <v>99</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="13" t="s">
+      <c r="H48" s="26"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L48" s="4" t="s">
@@ -2839,15 +2840,15 @@
       <c r="N48" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O48" s="17">
+      <c r="O48" s="16">
         <v>2000</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A49" s="24">
         <v>45</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -2863,22 +2864,22 @@
         <v>24</v>
       </c>
       <c r="G49" s="2"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="13"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="12"/>
       <c r="L49" s="4" t="s">
         <v>120</v>
       </c>
       <c r="M49" s="10"/>
       <c r="N49" s="11"/>
-      <c r="O49" s="17"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="25">
+      <c r="O49" s="16"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A50" s="24">
         <v>46</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -2894,22 +2895,22 @@
         <v>24</v>
       </c>
       <c r="G50" s="2"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="13"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="12"/>
       <c r="L50" s="4" t="s">
         <v>121</v>
       </c>
       <c r="M50" s="10"/>
       <c r="N50" s="11"/>
-      <c r="O50" s="17"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="25">
+      <c r="O50" s="16"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A51" s="24">
         <v>47</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -2925,10 +2926,10 @@
         <v>54</v>
       </c>
       <c r="G51" s="2"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="13" t="s">
+      <c r="H51" s="26"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L51" s="4" t="s">
@@ -2938,40 +2939,40 @@
       <c r="N51" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O51" s="17">
+      <c r="O51" s="16">
         <v>3000</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="25">
+    <row r="52" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="24">
         <v>48</v>
       </c>
-      <c r="B52" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" s="29" t="s">
+      <c r="B52" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="G52" s="29"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="21" t="s">
+      <c r="G52" s="28"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="M52" s="22"/>
-      <c r="N52" s="23"/>
-      <c r="O52" s="24"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>